<commit_message>
updated tech payroll Final. changed settings in Pycharm for file recognition of excel files
</commit_message>
<xml_diff>
--- a/XL_Files/Tech Payroll Final.xlsx
+++ b/XL_Files/Tech Payroll Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\total\Dropbox\TMB\accounting\Payroll Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git files to save backup_office\tmb_if\XL_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628399A2-DE09-4B93-B2BA-3104678085D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54DA4AC-A301-4887-9E05-77E6A108D025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="7170" windowWidth="29370" windowHeight="20700" activeTab="3" xr2:uid="{679A9B5C-2E5A-465E-8EDE-C1A09F9A5707}"/>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="25890" windowHeight="20970" activeTab="1" xr2:uid="{679A9B5C-2E5A-465E-8EDE-C1A09F9A5707}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll Master" sheetId="9" r:id="rId1"/>
@@ -19224,7 +19224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF849323-0637-42EF-9FA3-CB534CA174ED}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -19263,7 +19263,7 @@
       </c>
       <c r="J1" s="176">
         <f ca="1">TODAY()</f>
-        <v>44931</v>
+        <v>44932</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -19982,7 +19982,7 @@
   </sheetPr>
   <dimension ref="A1:CA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Z13" sqref="Z13:AC13"/>
     </sheetView>
@@ -21703,7 +21703,7 @@
         <v>106285.31</v>
       </c>
       <c r="AA17" s="111">
-        <f t="shared" ref="AA17:AB17" si="1">SUM(AA18+AA2)</f>
+        <f t="shared" ref="AA17" si="1">SUM(AA18+AA2)</f>
         <v>97378.349999999991</v>
       </c>
       <c r="AB17" s="111">

</xml_diff>